<commit_message>
Update CRONOGRAMA- AYRIHUANCA - 06.xlsx
</commit_message>
<xml_diff>
--- a/9.0 CRONOGRAMA/CRONOGRAMA- AYRIHUANCA - 06.xlsx
+++ b/9.0 CRONOGRAMA/CRONOGRAMA- AYRIHUANCA - 06.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\RepositorioORFEI\HIPOLITO PERSONAL\IOARR0006-AYRIHUANCA\9.0 CRONOGRAMA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\REPOSITORIO ORFEI\IOARR0006-AYRIHUANCA\9.0 CRONOGRAMA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F20D603-BDB7-439A-8008-EF9162D2E283}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B18E36D-2A91-43D6-A17D-25F55F5FD993}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15360" yWindow="0" windowWidth="15360" windowHeight="16680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FINANCIERO" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="0">FINANCIERO!$A$1:$F$18</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">FISICO!$A$1:$R$23</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -151,8 +151,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
-    <numFmt numFmtId="44" formatCode="_-&quot;S/.&quot;* #,##0.00_-;\-&quot;S/.&quot;* #,##0.00_-;_-&quot;S/.&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="_-&quot;S/&quot;* #,##0.00_-;\-&quot;S/&quot;* #,##0.00_-;_-&quot;S/&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;S/&quot;* #,##0.00_-;\-&quot;S/&quot;* #,##0.00_-;_-&quot;S/&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-&quot;S/.&quot;* #,##0.00_-;\-&quot;S/.&quot;* #,##0.00_-;_-&quot;S/.&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="_ &quot;S/&quot;\ * #,##0.00_ ;_ &quot;S/&quot;\ * \-#,##0.00_ ;_ &quot;S/&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="10" x14ac:knownFonts="1">
@@ -225,7 +225,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -241,12 +241,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFDDEBF7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF9BC2E6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -584,7 +578,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -597,140 +591,113 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="3" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="7" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="7" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="3" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="3" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="4" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="8" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="8" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="3" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="165" fontId="5" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -742,32 +709,65 @@
     <xf numFmtId="165" fontId="5" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="44" fontId="5" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="44" fontId="5" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="44" fontId="5" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="7" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="7" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="7" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="7" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1719,8 +1719,8 @@
   </sheetPr>
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScale="150" zoomScaleNormal="110" zoomScaleSheetLayoutView="150" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="150" zoomScaleNormal="110" zoomScaleSheetLayoutView="150" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -1735,296 +1735,296 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="39" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="47"/>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
-      <c r="F1" s="47"/>
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
+      <c r="F1" s="40"/>
     </row>
     <row r="2" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="36" t="s">
+      <c r="A2" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="36" t="s">
+      <c r="B2" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="36" t="s">
+      <c r="C2" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="36" t="s">
+      <c r="D2" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="36" t="s">
+      <c r="E2" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="36" t="s">
+      <c r="F2" s="31" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="14"/>
-      <c r="C3" s="15">
+      <c r="B3" s="13"/>
+      <c r="C3" s="14">
         <f>F3</f>
         <v>1781.55</v>
       </c>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="15">
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14">
         <v>1781.55</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="33" t="s">
+      <c r="A4" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="34"/>
-      <c r="C4" s="34"/>
-      <c r="D4" s="34"/>
-      <c r="E4" s="34"/>
-      <c r="F4" s="35"/>
+      <c r="B4" s="29"/>
+      <c r="C4" s="29"/>
+      <c r="D4" s="29"/>
+      <c r="E4" s="29"/>
+      <c r="F4" s="30"/>
     </row>
     <row r="5" spans="1:6" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="13" t="s">
+      <c r="A5" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="14"/>
-      <c r="C5" s="15">
+      <c r="B5" s="13"/>
+      <c r="C5" s="14">
         <v>105356.47</v>
       </c>
-      <c r="D5" s="15"/>
-      <c r="E5" s="15"/>
-      <c r="F5" s="15">
+      <c r="D5" s="14"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="14">
         <v>105356.47</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="13" t="s">
+      <c r="A6" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="14"/>
-      <c r="C6" s="15">
+      <c r="B6" s="13"/>
+      <c r="C6" s="14">
         <f>F6/2</f>
         <v>17726.25</v>
       </c>
-      <c r="D6" s="15">
+      <c r="D6" s="14">
         <f>F6/2</f>
         <v>17726.25</v>
       </c>
-      <c r="E6" s="15"/>
-      <c r="F6" s="15">
+      <c r="E6" s="14"/>
+      <c r="F6" s="14">
         <v>35452.5</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="16" t="s">
+      <c r="A7" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="14"/>
-      <c r="C7" s="15"/>
-      <c r="D7" s="15">
+      <c r="B7" s="13"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="14">
         <f>F7</f>
         <v>10718.26</v>
       </c>
-      <c r="E7" s="15"/>
-      <c r="F7" s="15">
+      <c r="E7" s="14"/>
+      <c r="F7" s="14">
         <v>10718.26</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="16" t="s">
+      <c r="A8" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="14"/>
-      <c r="C8" s="15"/>
-      <c r="D8" s="15">
+      <c r="B8" s="13"/>
+      <c r="C8" s="14"/>
+      <c r="D8" s="14">
         <f>F8</f>
         <v>5124.82</v>
       </c>
-      <c r="E8" s="15"/>
-      <c r="F8" s="15">
+      <c r="E8" s="14"/>
+      <c r="F8" s="14">
         <v>5124.82</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="13" t="s">
+      <c r="A9" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="14"/>
-      <c r="C9" s="15">
+      <c r="B9" s="13"/>
+      <c r="C9" s="14">
         <f>F9</f>
         <v>3500</v>
       </c>
-      <c r="D9" s="15"/>
-      <c r="E9" s="17"/>
-      <c r="F9" s="18">
+      <c r="D9" s="14"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="17">
         <v>3500</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="19" t="s">
+      <c r="A10" s="59" t="s">
         <v>32</v>
       </c>
-      <c r="B10" s="20"/>
-      <c r="C10" s="21">
+      <c r="B10" s="60"/>
+      <c r="C10" s="61">
         <f>SUM(C3:C9)</f>
         <v>128364.27</v>
       </c>
-      <c r="D10" s="21">
+      <c r="D10" s="61">
         <f>SUM(D3:D9)</f>
         <v>33569.33</v>
       </c>
-      <c r="E10" s="22"/>
-      <c r="F10" s="23">
+      <c r="E10" s="62"/>
+      <c r="F10" s="63">
         <f>F3+F5+F6+F7+F8+F9</f>
         <v>161933.60000000003</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="13" t="s">
+      <c r="A11" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="24"/>
-      <c r="C11" s="25">
+      <c r="B11" s="20"/>
+      <c r="C11" s="21">
         <f>F11/2</f>
         <v>31508.89</v>
       </c>
-      <c r="D11" s="25">
+      <c r="D11" s="21">
         <f>F11/2</f>
         <v>31508.89</v>
       </c>
-      <c r="E11" s="26"/>
-      <c r="F11" s="27">
+      <c r="E11" s="22"/>
+      <c r="F11" s="23">
         <v>63017.78</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="13" t="s">
+      <c r="A12" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="24"/>
-      <c r="C12" s="25">
+      <c r="B12" s="20"/>
+      <c r="C12" s="21">
         <f>F12/2</f>
         <v>7732.03</v>
       </c>
-      <c r="D12" s="25">
+      <c r="D12" s="21">
         <f>F12/2</f>
         <v>7732.03</v>
       </c>
-      <c r="E12" s="25"/>
-      <c r="F12" s="27">
+      <c r="E12" s="21"/>
+      <c r="F12" s="23">
         <v>15464.06</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="42" t="s">
+      <c r="A13" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="B13" s="38"/>
-      <c r="C13" s="39"/>
-      <c r="D13" s="39"/>
-      <c r="E13" s="40"/>
-      <c r="F13" s="40">
+      <c r="B13" s="33"/>
+      <c r="C13" s="34"/>
+      <c r="D13" s="34"/>
+      <c r="E13" s="35"/>
+      <c r="F13" s="35">
         <f>F10+F11+F12</f>
         <v>240415.44000000003</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="28" t="s">
+      <c r="A14" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="29"/>
-      <c r="C14" s="25">
+      <c r="B14" s="25"/>
+      <c r="C14" s="21">
         <f>F14/2</f>
         <v>12480.75</v>
       </c>
-      <c r="D14" s="25">
+      <c r="D14" s="21">
         <f>F14/2</f>
         <v>12480.75</v>
       </c>
-      <c r="E14" s="25"/>
-      <c r="F14" s="27">
+      <c r="E14" s="21"/>
+      <c r="F14" s="23">
         <v>24961.5</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="13" t="s">
+      <c r="A15" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B15" s="15">
+      <c r="B15" s="14">
         <f>F15</f>
         <v>10000</v>
       </c>
-      <c r="C15" s="15"/>
-      <c r="D15" s="15"/>
-      <c r="E15" s="15"/>
-      <c r="F15" s="27">
+      <c r="C15" s="14"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="23">
         <v>10000</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="13" t="s">
+      <c r="A16" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="B16" s="15"/>
-      <c r="C16" s="15"/>
-      <c r="D16" s="15"/>
-      <c r="E16" s="15">
+      <c r="B16" s="14"/>
+      <c r="C16" s="14"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="14">
         <f>F16</f>
         <v>17290.75</v>
       </c>
-      <c r="F16" s="30">
+      <c r="F16" s="26">
         <v>17290.75</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="19" t="s">
+      <c r="A17" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="B17" s="31">
+      <c r="B17" s="27">
         <f>SUM(B10:B16)</f>
         <v>10000</v>
       </c>
-      <c r="C17" s="31">
+      <c r="C17" s="27">
         <f>SUM(C10:C16)</f>
         <v>180085.94</v>
       </c>
-      <c r="D17" s="31">
+      <c r="D17" s="27">
         <f>SUM(D10:D16)</f>
         <v>85291</v>
       </c>
-      <c r="E17" s="31">
+      <c r="E17" s="27">
         <f>SUM(E10:E16)</f>
         <v>17290.75</v>
       </c>
-      <c r="F17" s="41">
+      <c r="F17" s="36">
         <f>SUM(F14:F16)</f>
         <v>52252.25</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="43" t="s">
+      <c r="A18" s="55" t="s">
         <v>12</v>
       </c>
-      <c r="B18" s="44"/>
-      <c r="C18" s="44"/>
-      <c r="D18" s="44"/>
-      <c r="E18" s="45"/>
-      <c r="F18" s="32">
+      <c r="B18" s="56"/>
+      <c r="C18" s="56"/>
+      <c r="D18" s="56"/>
+      <c r="E18" s="57"/>
+      <c r="F18" s="58">
         <f>+F13+F17+0.01</f>
         <v>292667.70000000007</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D20" s="37"/>
+      <c r="D20" s="32"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D21" s="37"/>
+      <c r="D21" s="32"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2044,8 +2044,8 @@
   </sheetPr>
   <dimension ref="A1:R20"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="118" zoomScaleNormal="110" zoomScaleSheetLayoutView="118" workbookViewId="0">
-      <selection activeCell="R14" sqref="R14"/>
+    <sheetView view="pageBreakPreview" zoomScale="118" zoomScaleNormal="110" zoomScaleSheetLayoutView="118" workbookViewId="0">
+      <selection activeCell="L22" sqref="L22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -2057,110 +2057,110 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="61.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="41" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
-      <c r="G1" s="50"/>
-      <c r="H1" s="50"/>
-      <c r="I1" s="50"/>
-      <c r="J1" s="50"/>
-      <c r="K1" s="50"/>
-      <c r="L1" s="50"/>
-      <c r="M1" s="50"/>
-      <c r="N1" s="50"/>
-      <c r="O1" s="50"/>
-      <c r="P1" s="50"/>
-      <c r="Q1" s="50"/>
-      <c r="R1" s="50"/>
+      <c r="B1" s="41"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
+      <c r="I1" s="41"/>
+      <c r="J1" s="41"/>
+      <c r="K1" s="41"/>
+      <c r="L1" s="41"/>
+      <c r="M1" s="41"/>
+      <c r="N1" s="41"/>
+      <c r="O1" s="41"/>
+      <c r="P1" s="41"/>
+      <c r="Q1" s="41"/>
+      <c r="R1" s="41"/>
     </row>
     <row r="2" spans="1:18" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="51" t="s">
+      <c r="A2" s="42" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="49" t="s">
+      <c r="B2" s="54" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="49"/>
-      <c r="D2" s="49"/>
-      <c r="E2" s="49"/>
-      <c r="F2" s="49" t="s">
+      <c r="C2" s="54"/>
+      <c r="D2" s="54"/>
+      <c r="E2" s="54"/>
+      <c r="F2" s="54" t="s">
         <v>24</v>
       </c>
-      <c r="G2" s="49"/>
-      <c r="H2" s="49"/>
-      <c r="I2" s="49"/>
-      <c r="J2" s="49" t="s">
+      <c r="G2" s="54"/>
+      <c r="H2" s="54"/>
+      <c r="I2" s="54"/>
+      <c r="J2" s="54" t="s">
         <v>25</v>
       </c>
-      <c r="K2" s="49"/>
-      <c r="L2" s="49"/>
-      <c r="M2" s="49"/>
-      <c r="N2" s="49" t="s">
+      <c r="K2" s="54"/>
+      <c r="L2" s="54"/>
+      <c r="M2" s="54"/>
+      <c r="N2" s="54" t="s">
         <v>26</v>
       </c>
-      <c r="O2" s="49"/>
-      <c r="P2" s="49"/>
-      <c r="Q2" s="49"/>
-      <c r="R2" s="9" t="s">
+      <c r="O2" s="54"/>
+      <c r="P2" s="54"/>
+      <c r="Q2" s="54"/>
+      <c r="R2" s="8" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:18" s="2" customFormat="1" ht="10.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="51"/>
-      <c r="B3" s="9" t="s">
+      <c r="A3" s="42"/>
+      <c r="B3" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="E3" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="F3" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="G3" s="9" t="s">
+      <c r="G3" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="H3" s="9" t="s">
+      <c r="H3" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="I3" s="9" t="s">
+      <c r="I3" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="J3" s="9" t="s">
+      <c r="J3" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="K3" s="9" t="s">
+      <c r="K3" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="L3" s="9" t="s">
+      <c r="L3" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="M3" s="9" t="s">
+      <c r="M3" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="N3" s="9" t="s">
+      <c r="N3" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="O3" s="9" t="s">
+      <c r="O3" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="P3" s="9" t="s">
+      <c r="P3" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="Q3" s="9" t="s">
+      <c r="Q3" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="R3" s="9"/>
+      <c r="R3" s="8"/>
     </row>
     <row r="4" spans="1:18" s="2" customFormat="1" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
@@ -2170,10 +2170,10 @@
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10"/>
-      <c r="H4" s="10"/>
-      <c r="I4" s="10"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="9"/>
       <c r="J4" s="3"/>
       <c r="K4" s="3"/>
       <c r="L4" s="3"/>
@@ -2182,31 +2182,31 @@
       <c r="O4" s="3"/>
       <c r="P4" s="3"/>
       <c r="Q4" s="3"/>
-      <c r="R4" s="15">
+      <c r="R4" s="14">
         <v>1781.55</v>
       </c>
     </row>
     <row r="5" spans="1:18" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="60" t="s">
+      <c r="A5" s="51" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="61"/>
-      <c r="C5" s="61"/>
-      <c r="D5" s="61"/>
-      <c r="E5" s="61"/>
-      <c r="F5" s="61"/>
-      <c r="G5" s="61"/>
-      <c r="H5" s="61"/>
-      <c r="I5" s="61"/>
-      <c r="J5" s="61"/>
-      <c r="K5" s="61"/>
-      <c r="L5" s="61"/>
-      <c r="M5" s="61"/>
-      <c r="N5" s="61"/>
-      <c r="O5" s="61"/>
-      <c r="P5" s="61"/>
-      <c r="Q5" s="61"/>
-      <c r="R5" s="62"/>
+      <c r="B5" s="52"/>
+      <c r="C5" s="52"/>
+      <c r="D5" s="52"/>
+      <c r="E5" s="52"/>
+      <c r="F5" s="52"/>
+      <c r="G5" s="52"/>
+      <c r="H5" s="52"/>
+      <c r="I5" s="52"/>
+      <c r="J5" s="52"/>
+      <c r="K5" s="52"/>
+      <c r="L5" s="52"/>
+      <c r="M5" s="52"/>
+      <c r="N5" s="52"/>
+      <c r="O5" s="52"/>
+      <c r="P5" s="52"/>
+      <c r="Q5" s="52"/>
+      <c r="R5" s="53"/>
     </row>
     <row r="6" spans="1:18" s="2" customFormat="1" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
@@ -2216,10 +2216,10 @@
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="10"/>
-      <c r="I6" s="10"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9"/>
       <c r="J6" s="3"/>
       <c r="K6" s="3"/>
       <c r="L6" s="3"/>
@@ -2228,7 +2228,7 @@
       <c r="O6" s="3"/>
       <c r="P6" s="3"/>
       <c r="Q6" s="3"/>
-      <c r="R6" s="15">
+      <c r="R6" s="14">
         <v>105356.47</v>
       </c>
     </row>
@@ -2240,19 +2240,19 @@
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
-      <c r="F7" s="10"/>
-      <c r="G7" s="10"/>
-      <c r="H7" s="10"/>
-      <c r="I7" s="10"/>
-      <c r="J7" s="10"/>
-      <c r="K7" s="10"/>
-      <c r="L7" s="10"/>
-      <c r="M7" s="10"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="9"/>
+      <c r="J7" s="9"/>
+      <c r="K7" s="9"/>
+      <c r="L7" s="9"/>
+      <c r="M7" s="9"/>
       <c r="N7" s="3"/>
       <c r="O7" s="3"/>
       <c r="P7" s="3"/>
       <c r="Q7" s="3"/>
-      <c r="R7" s="15">
+      <c r="R7" s="14">
         <v>35452.5</v>
       </c>
     </row>
@@ -2268,15 +2268,15 @@
       <c r="G8" s="4"/>
       <c r="H8" s="4"/>
       <c r="I8" s="4"/>
-      <c r="J8" s="11"/>
-      <c r="K8" s="11"/>
-      <c r="L8" s="11"/>
-      <c r="M8" s="11"/>
+      <c r="J8" s="10"/>
+      <c r="K8" s="10"/>
+      <c r="L8" s="10"/>
+      <c r="M8" s="10"/>
       <c r="N8" s="4"/>
       <c r="O8" s="4"/>
       <c r="P8" s="4"/>
       <c r="Q8" s="4"/>
-      <c r="R8" s="15">
+      <c r="R8" s="14">
         <v>10718.26</v>
       </c>
     </row>
@@ -2292,15 +2292,15 @@
       <c r="G9" s="4"/>
       <c r="H9" s="4"/>
       <c r="I9" s="4"/>
-      <c r="J9" s="11"/>
-      <c r="K9" s="11"/>
-      <c r="L9" s="11"/>
-      <c r="M9" s="11"/>
+      <c r="J9" s="10"/>
+      <c r="K9" s="10"/>
+      <c r="L9" s="10"/>
+      <c r="M9" s="10"/>
       <c r="N9" s="4"/>
       <c r="O9" s="4"/>
       <c r="P9" s="4"/>
       <c r="Q9" s="4"/>
-      <c r="R9" s="15">
+      <c r="R9" s="14">
         <v>5124.82</v>
       </c>
     </row>
@@ -2312,10 +2312,10 @@
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="10"/>
-      <c r="H10" s="10"/>
-      <c r="I10" s="10"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="9"/>
       <c r="J10" s="3"/>
       <c r="K10" s="3"/>
       <c r="L10" s="3"/>
@@ -2324,7 +2324,7 @@
       <c r="O10" s="3"/>
       <c r="P10" s="3"/>
       <c r="Q10" s="3"/>
-      <c r="R10" s="18">
+      <c r="R10" s="17">
         <v>3500</v>
       </c>
     </row>
@@ -2348,7 +2348,7 @@
       <c r="O11" s="6"/>
       <c r="P11" s="6"/>
       <c r="Q11" s="6"/>
-      <c r="R11" s="23">
+      <c r="R11" s="19">
         <f>R4+R6+R7+R8+R9+R10</f>
         <v>161933.60000000003</v>
       </c>
@@ -2361,19 +2361,19 @@
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
-      <c r="F12" s="10"/>
-      <c r="G12" s="10"/>
-      <c r="H12" s="10"/>
-      <c r="I12" s="10"/>
-      <c r="J12" s="10"/>
-      <c r="K12" s="10"/>
-      <c r="L12" s="10"/>
-      <c r="M12" s="10"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="9"/>
+      <c r="I12" s="9"/>
+      <c r="J12" s="9"/>
+      <c r="K12" s="9"/>
+      <c r="L12" s="9"/>
+      <c r="M12" s="9"/>
       <c r="N12" s="3"/>
       <c r="O12" s="3"/>
       <c r="P12" s="3"/>
       <c r="Q12" s="3"/>
-      <c r="R12" s="27">
+      <c r="R12" s="23">
         <v>63017.78</v>
       </c>
     </row>
@@ -2385,43 +2385,43 @@
       <c r="C13" s="5"/>
       <c r="D13" s="5"/>
       <c r="E13" s="5"/>
-      <c r="F13" s="10"/>
-      <c r="G13" s="10"/>
-      <c r="H13" s="10"/>
-      <c r="I13" s="10"/>
-      <c r="J13" s="10"/>
-      <c r="K13" s="10"/>
-      <c r="L13" s="10"/>
-      <c r="M13" s="10"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="9"/>
+      <c r="I13" s="9"/>
+      <c r="J13" s="9"/>
+      <c r="K13" s="9"/>
+      <c r="L13" s="9"/>
+      <c r="M13" s="9"/>
       <c r="N13" s="5"/>
       <c r="O13" s="5"/>
       <c r="P13" s="5"/>
       <c r="Q13" s="5"/>
-      <c r="R13" s="27">
+      <c r="R13" s="23">
         <v>15464.06</v>
       </c>
     </row>
     <row r="14" spans="1:18" s="2" customFormat="1" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="42" t="s">
+      <c r="A14" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="B14" s="63"/>
-      <c r="C14" s="63"/>
-      <c r="D14" s="63"/>
-      <c r="E14" s="63"/>
-      <c r="F14" s="63"/>
-      <c r="G14" s="63"/>
-      <c r="H14" s="63"/>
-      <c r="I14" s="63"/>
-      <c r="J14" s="63"/>
-      <c r="K14" s="63"/>
-      <c r="L14" s="63"/>
-      <c r="M14" s="63"/>
-      <c r="N14" s="63"/>
-      <c r="O14" s="63"/>
-      <c r="P14" s="63"/>
-      <c r="Q14" s="63"/>
-      <c r="R14" s="26">
+      <c r="B14" s="38"/>
+      <c r="C14" s="38"/>
+      <c r="D14" s="38"/>
+      <c r="E14" s="38"/>
+      <c r="F14" s="38"/>
+      <c r="G14" s="38"/>
+      <c r="H14" s="38"/>
+      <c r="I14" s="38"/>
+      <c r="J14" s="38"/>
+      <c r="K14" s="38"/>
+      <c r="L14" s="38"/>
+      <c r="M14" s="38"/>
+      <c r="N14" s="38"/>
+      <c r="O14" s="38"/>
+      <c r="P14" s="38"/>
+      <c r="Q14" s="38"/>
+      <c r="R14" s="22">
         <f>R11+R12+R13</f>
         <v>240415.44000000003</v>
       </c>
@@ -2434,19 +2434,19 @@
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
       <c r="E15" s="5"/>
-      <c r="F15" s="10"/>
-      <c r="G15" s="10"/>
-      <c r="H15" s="10"/>
-      <c r="I15" s="10"/>
-      <c r="J15" s="10"/>
-      <c r="K15" s="10"/>
-      <c r="L15" s="10"/>
-      <c r="M15" s="10"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="9"/>
+      <c r="I15" s="9"/>
+      <c r="J15" s="9"/>
+      <c r="K15" s="9"/>
+      <c r="L15" s="9"/>
+      <c r="M15" s="9"/>
       <c r="N15" s="5"/>
       <c r="O15" s="5"/>
       <c r="P15" s="5"/>
       <c r="Q15" s="5"/>
-      <c r="R15" s="27">
+      <c r="R15" s="23">
         <v>24961.5</v>
       </c>
     </row>
@@ -2454,10 +2454,10 @@
       <c r="A16" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B16" s="10"/>
-      <c r="C16" s="10"/>
-      <c r="D16" s="10"/>
-      <c r="E16" s="10"/>
+      <c r="B16" s="9"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9"/>
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
       <c r="H16" s="3"/>
@@ -2470,7 +2470,7 @@
       <c r="O16" s="3"/>
       <c r="P16" s="3"/>
       <c r="Q16" s="3"/>
-      <c r="R16" s="27">
+      <c r="R16" s="23">
         <v>10000</v>
       </c>
     </row>
@@ -2490,16 +2490,16 @@
       <c r="K17" s="3"/>
       <c r="L17" s="3"/>
       <c r="M17" s="3"/>
-      <c r="N17" s="10"/>
-      <c r="O17" s="10"/>
-      <c r="P17" s="10"/>
-      <c r="Q17" s="10"/>
-      <c r="R17" s="30">
+      <c r="N17" s="9"/>
+      <c r="O17" s="9"/>
+      <c r="P17" s="9"/>
+      <c r="Q17" s="9"/>
+      <c r="R17" s="26">
         <v>17290.75</v>
       </c>
     </row>
     <row r="18" spans="1:18" s="2" customFormat="1" ht="3.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="58" t="s">
+      <c r="A18" s="49" t="s">
         <v>7</v>
       </c>
       <c r="B18" s="6"/>
@@ -2518,67 +2518,72 @@
       <c r="O18" s="6"/>
       <c r="P18" s="6"/>
       <c r="Q18" s="6"/>
-      <c r="R18" s="8"/>
+      <c r="R18" s="7"/>
     </row>
     <row r="19" spans="1:18" s="2" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="59"/>
-      <c r="B19" s="52">
+      <c r="A19" s="50"/>
+      <c r="B19" s="43">
         <f>FINANCIERO!B17</f>
         <v>10000</v>
       </c>
-      <c r="C19" s="53"/>
-      <c r="D19" s="53"/>
-      <c r="E19" s="54"/>
-      <c r="F19" s="55">
+      <c r="C19" s="44"/>
+      <c r="D19" s="44"/>
+      <c r="E19" s="45"/>
+      <c r="F19" s="46">
         <f>FINANCIERO!C17</f>
         <v>180085.94</v>
       </c>
-      <c r="G19" s="56"/>
-      <c r="H19" s="56"/>
-      <c r="I19" s="57"/>
-      <c r="J19" s="55">
+      <c r="G19" s="47"/>
+      <c r="H19" s="47"/>
+      <c r="I19" s="48"/>
+      <c r="J19" s="46">
         <f>FINANCIERO!D17</f>
         <v>85291</v>
       </c>
-      <c r="K19" s="56"/>
-      <c r="L19" s="56"/>
-      <c r="M19" s="57"/>
-      <c r="N19" s="55">
+      <c r="K19" s="47"/>
+      <c r="L19" s="47"/>
+      <c r="M19" s="48"/>
+      <c r="N19" s="46">
         <f>FINANCIERO!E17</f>
         <v>17290.75</v>
       </c>
-      <c r="O19" s="56"/>
-      <c r="P19" s="56"/>
-      <c r="Q19" s="57"/>
-      <c r="R19" s="12"/>
-    </row>
-    <row r="20" spans="1:18" s="2" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A20" s="48" t="s">
+      <c r="O19" s="47"/>
+      <c r="P19" s="47"/>
+      <c r="Q19" s="48"/>
+      <c r="R19" s="11"/>
+    </row>
+    <row r="20" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="64" t="s">
         <v>12</v>
       </c>
-      <c r="B20" s="48"/>
-      <c r="C20" s="48"/>
-      <c r="D20" s="48"/>
-      <c r="E20" s="48"/>
-      <c r="F20" s="48"/>
-      <c r="G20" s="48"/>
-      <c r="H20" s="48"/>
-      <c r="I20" s="48"/>
-      <c r="J20" s="48"/>
-      <c r="K20" s="48"/>
-      <c r="L20" s="48"/>
-      <c r="M20" s="48"/>
-      <c r="N20" s="48"/>
-      <c r="O20" s="48"/>
-      <c r="P20" s="48"/>
-      <c r="Q20" s="48"/>
-      <c r="R20" s="7">
+      <c r="B20" s="64"/>
+      <c r="C20" s="64"/>
+      <c r="D20" s="64"/>
+      <c r="E20" s="64"/>
+      <c r="F20" s="64"/>
+      <c r="G20" s="64"/>
+      <c r="H20" s="64"/>
+      <c r="I20" s="64"/>
+      <c r="J20" s="64"/>
+      <c r="K20" s="64"/>
+      <c r="L20" s="64"/>
+      <c r="M20" s="64"/>
+      <c r="N20" s="64"/>
+      <c r="O20" s="64"/>
+      <c r="P20" s="64"/>
+      <c r="Q20" s="64"/>
+      <c r="R20" s="65">
         <f>R14+R15+R16+R17+0.01</f>
         <v>292667.70000000007</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A20:Q20"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="F2:I2"/>
+    <mergeCell ref="J2:M2"/>
+    <mergeCell ref="N2:Q2"/>
     <mergeCell ref="A1:R1"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="B19:E19"/>
@@ -2587,11 +2592,6 @@
     <mergeCell ref="N19:Q19"/>
     <mergeCell ref="A18:A19"/>
     <mergeCell ref="A5:R5"/>
-    <mergeCell ref="A20:Q20"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="F2:I2"/>
-    <mergeCell ref="J2:M2"/>
-    <mergeCell ref="N2:Q2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="99" fitToHeight="0" orientation="portrait" r:id="rId1"/>

</xml_diff>